<commit_message>
Paranoid Push of BOM (WIP)
</commit_message>
<xml_diff>
--- a/Eagle/Schematics & Board Layout/Tx Board Schematic/T08-TxClicker_BOM.xlsx
+++ b/Eagle/Schematics & Board Layout/Tx Board Schematic/T08-TxClicker_BOM.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="T08-TxClicker" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="178">
   <si>
     <t>Qty</t>
   </si>
@@ -67,9 +67,6 @@
     <t>R6</t>
   </si>
   <si>
-    <t>RESISTOR, American symbol</t>
-  </si>
-  <si>
     <t>1.5pF</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
     <t>C3, C5, C10, C12, C15, C16, C18, C20, C21</t>
   </si>
   <si>
-    <t>CAPACITOR, European symbol</t>
-  </si>
-  <si>
     <t>100pF</t>
   </si>
   <si>
@@ -190,12 +184,6 @@
     <t>2pF</t>
   </si>
   <si>
-    <t>C17, C19</t>
-  </si>
-  <si>
-    <t>C6, C7, C8</t>
-  </si>
-  <si>
     <t>3.3k</t>
   </si>
   <si>
@@ -364,9 +352,6 @@
     <t>Unit Price</t>
   </si>
   <si>
-    <t>100x Price</t>
-  </si>
-  <si>
     <t>160-1183-1-ND</t>
   </si>
   <si>
@@ -380,13 +365,196 @@
   </si>
   <si>
     <t>LTST-C190GKT</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>OSH PARK Board</t>
+  </si>
+  <si>
+    <t>478-6712-1-ND</t>
+  </si>
+  <si>
+    <t>Extended Price @100x</t>
+  </si>
+  <si>
+    <t>AVX Corporation</t>
+  </si>
+  <si>
+    <t>ML03511R5BAT2A</t>
+  </si>
+  <si>
+    <t>CAP CER MLO 1.5PF 50V NP0 0603</t>
+  </si>
+  <si>
+    <t>399-5089-1-ND</t>
+  </si>
+  <si>
+    <t>C0603C104K5RACTU</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 50V 10% X7R 0603</t>
+  </si>
+  <si>
+    <t>Kemet</t>
+  </si>
+  <si>
+    <t>399-7819-1-ND</t>
+  </si>
+  <si>
+    <t>C0603C101F5GACTU</t>
+  </si>
+  <si>
+    <t>CAP CER 100PF 50V 1% NP0 0603</t>
+  </si>
+  <si>
+    <t>587-3238-1-ND</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
+  </si>
+  <si>
+    <t>EMK107BBJ106MA-T</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 16V 20% X5R 0603</t>
+  </si>
+  <si>
+    <t>1276-2204-1-ND</t>
+  </si>
+  <si>
+    <t>CL10C160JB8NNNC</t>
+  </si>
+  <si>
+    <t>CAP CER 16PF 50V 5% NP0 0603</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics America, Inc</t>
+  </si>
+  <si>
+    <t>478-6732-1-ND</t>
+  </si>
+  <si>
+    <t>ML03511R0AAT2A</t>
+  </si>
+  <si>
+    <t>CAP CER MLO 1PF 50V NP0 0603</t>
+  </si>
+  <si>
+    <t>CAP CER 2000PF 50V 5% NP0 0603</t>
+  </si>
+  <si>
+    <t>490-1458-1-ND</t>
+  </si>
+  <si>
+    <t>Murata Electronics North America</t>
+  </si>
+  <si>
+    <t>GRM1885C1H202JA01D</t>
+  </si>
+  <si>
+    <t>C6, C7, C8, C17, C19</t>
+  </si>
+  <si>
+    <t>CAP CER MLO 2PF 50V NP0 0603</t>
+  </si>
+  <si>
+    <t>478-6717-1-ND</t>
+  </si>
+  <si>
+    <t>ML03512R0BAT2A</t>
+  </si>
+  <si>
+    <t>587-3171-1-ND</t>
+  </si>
+  <si>
+    <t>UMK107ABJ474KA-T</t>
+  </si>
+  <si>
+    <t>CAP CER 0.47UF 50V 10% X5R 0603</t>
+  </si>
+  <si>
+    <t>490-3567-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 8.2PF 50V NP0 0603</t>
+  </si>
+  <si>
+    <t>GQM1885C1H8R2CB01D</t>
+  </si>
+  <si>
+    <t>BHSD-2032-SMCT-ND</t>
+  </si>
+  <si>
+    <t>MPD (Memory Protection Devices)</t>
+  </si>
+  <si>
+    <t>BHSD-2032-SM</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>RHM0.0CGCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rohm Semiconductor </t>
+  </si>
+  <si>
+    <t>MCR03ERTJ000</t>
+  </si>
+  <si>
+    <t>RES 0.0 OHM 1/10W JUMP 0603 SMD</t>
+  </si>
+  <si>
+    <t>RMCF0603FT10K0CT-ND</t>
+  </si>
+  <si>
+    <t>RES 10K OHM 1/10W 1% 0603</t>
+  </si>
+  <si>
+    <t>RMCF0603FT10K0</t>
+  </si>
+  <si>
+    <t>Stackpole Electronics Inc</t>
+  </si>
+  <si>
+    <t>RES 47K OHM 1/10W 1% 0603</t>
+  </si>
+  <si>
+    <t>RMCF0603FT47K0CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603FT47K0</t>
+  </si>
+  <si>
+    <t>RMCF0603FT56K0CT-ND</t>
+  </si>
+  <si>
+    <t>RES 56K OHM 1/10W 1% 0603</t>
+  </si>
+  <si>
+    <t>RMCF0603FT56K0</t>
+  </si>
+  <si>
+    <t>RES ARRAY 10K OHM 4 RES 2012</t>
+  </si>
+  <si>
+    <t>MNR34103CT-ND</t>
+  </si>
+  <si>
+    <t>MNR34J5ABJ103</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -541,6 +709,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -906,17 +1093,23 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -963,7 +1156,11 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -974,9 +1171,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:K43" totalsRowShown="0">
-  <autoFilter ref="A3:K43"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:L43" totalsRowShown="0">
+  <autoFilter ref="A3:L43">
+    <filterColumn colId="11">
+      <filters>
+        <filter val="0"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="12">
     <tableColumn id="1" name="Qty"/>
     <tableColumn id="2" name="Value"/>
     <tableColumn id="3" name="Device"/>
@@ -984,10 +1187,13 @@
     <tableColumn id="5" name="Parts"/>
     <tableColumn id="6" name="Description"/>
     <tableColumn id="7" name="Digikey#"/>
+    <tableColumn id="13" name="Manufacturer"/>
+    <tableColumn id="14" name="Manufacturer P/N"/>
     <tableColumn id="8" name="Unit Price"/>
-    <tableColumn id="9" name="100x Price"/>
-    <tableColumn id="10" name="Manufacturer"/>
-    <tableColumn id="11" name="Manufacturer P/N"/>
+    <tableColumn id="9" name="Extended Price @100x"/>
+    <tableColumn id="10" name="Total Cost" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1280,24 +1486,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:K43"/>
+  <dimension ref="A3:L45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
+    <col min="6" max="6" width="36.5703125" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="11" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="10" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1317,54 +1527,61 @@
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H3" t="s">
+        <v>113</v>
+      </c>
+      <c r="I3" t="s">
         <v>115</v>
       </c>
-      <c r="I3" t="s">
-        <v>116</v>
-      </c>
       <c r="J3" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="K3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="L3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H4">
+      <c r="G4" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="J4" s="3">
         <v>0.28000000000000003</v>
       </c>
-      <c r="I4">
+      <c r="K4" s="3">
         <v>0.1188</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1380,8 +1597,12 @@
       <c r="F5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1397,70 +1618,152 @@
       <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="H6" t="s">
+        <v>162</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J6">
+        <v>0.1</v>
+      </c>
+      <c r="K6">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="L6">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F7" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.27629999999999999</v>
+      </c>
+      <c r="L7">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9</v>
       </c>
       <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F8" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K8" s="3">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="L8">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.39</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="L9">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
@@ -1469,368 +1772,628 @@
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="H10" t="s">
+        <v>168</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J10">
+        <v>0.1</v>
+      </c>
+      <c r="K10">
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="L10">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
         <v>29</v>
       </c>
-      <c r="D11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="H11" t="s">
+        <v>162</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J11">
+        <v>0.3</v>
+      </c>
+      <c r="K11">
+        <v>9.8400000000000001E-2</v>
+      </c>
+      <c r="L11">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.49</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0.2142</v>
+      </c>
+      <c r="L12">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
         <v>35</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>36</v>
       </c>
-      <c r="D13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="L14">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="K15" s="3">
+        <v>3.0800000000000001E-2</v>
+      </c>
+      <c r="L15">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="L16">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" t="s">
         <v>30</v>
       </c>
-      <c r="E18" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="L19">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="L20">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="K21" s="3">
+        <v>4.2799999999999998E-2</v>
+      </c>
+      <c r="L21">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
         <v>55</v>
       </c>
-      <c r="C21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0.27629999999999999</v>
+      </c>
+      <c r="L22">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" t="s">
         <v>57</v>
       </c>
-      <c r="C22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" t="s">
-        <v>58</v>
-      </c>
-      <c r="F22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>30</v>
+      </c>
+      <c r="L23">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" t="s">
-        <v>61</v>
-      </c>
-      <c r="F24" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="J24" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="K24" s="3">
+        <v>3.8100000000000002E-2</v>
+      </c>
+      <c r="L24">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H25" t="s">
+        <v>168</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="J25">
+        <v>0.1</v>
+      </c>
+      <c r="K25">
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="L25">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E26" t="s">
-        <v>65</v>
-      </c>
-      <c r="F26" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="L26">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="J27">
+        <v>0.1</v>
+      </c>
+      <c r="K27">
+        <v>1.0500000000000001E-2</v>
+      </c>
+      <c r="L27">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" t="s">
-        <v>69</v>
-      </c>
-      <c r="F28" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0.2848</v>
+      </c>
+      <c r="L28">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" t="s">
         <v>70</v>
-      </c>
-      <c r="C29" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" t="s">
-        <v>19</v>
       </c>
       <c r="E29" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>72</v>
+      </c>
+      <c r="L29">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C30" t="s">
         <v>73</v>
@@ -1844,8 +2407,12 @@
       <c r="F30" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1855,25 +2422,44 @@
       <c r="C31" t="s">
         <v>77</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="K31" s="3">
+        <v>0.78749999999999998</v>
+      </c>
+      <c r="L31">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
-        <v>81</v>
-      </c>
       <c r="C32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D32" t="s">
         <v>81</v>
@@ -1884,68 +2470,78 @@
       <c r="F32" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B33" t="s">
         <v>84</v>
       </c>
       <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" t="s">
+        <v>85</v>
+      </c>
+      <c r="L33">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34" t="s">
         <v>84</v>
       </c>
-      <c r="D33" t="s">
-        <v>85</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" t="s">
         <v>86</v>
       </c>
-      <c r="F33" t="s">
+      <c r="L34">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>5</v>
-      </c>
-      <c r="B34" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" t="s">
-        <v>19</v>
-      </c>
-      <c r="E34" t="s">
-        <v>89</v>
-      </c>
-      <c r="F34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>2</v>
-      </c>
-      <c r="B35" t="s">
-        <v>88</v>
-      </c>
-      <c r="C35" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" t="s">
-        <v>90</v>
-      </c>
       <c r="F35" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="L35">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1953,81 +2549,97 @@
         <v>88</v>
       </c>
       <c r="C36" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E36" t="s">
-        <v>91</v>
-      </c>
-      <c r="F36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="L36">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" t="s">
         <v>92</v>
       </c>
-      <c r="C37" t="s">
-        <v>36</v>
-      </c>
-      <c r="D37" t="s">
-        <v>37</v>
-      </c>
-      <c r="E37" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L37">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
       <c r="B38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" t="s">
         <v>94</v>
       </c>
-      <c r="C38" t="s">
-        <v>94</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>95</v>
       </c>
-      <c r="E38" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L38">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
       <c r="B39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" t="s">
+        <v>96</v>
+      </c>
+      <c r="D39">
+        <v>603</v>
+      </c>
+      <c r="E39" t="s">
         <v>97</v>
       </c>
-      <c r="C39" t="s">
-        <v>97</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="F39" t="s">
         <v>98</v>
       </c>
-      <c r="E39" t="s">
+      <c r="L39">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" t="s">
         <v>100</v>
-      </c>
-      <c r="C40" t="s">
-        <v>100</v>
-      </c>
-      <c r="D40">
-        <v>603</v>
       </c>
       <c r="E40" t="s">
         <v>101</v>
@@ -2035,33 +2647,41 @@
       <c r="F40" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>103</v>
+      </c>
+      <c r="L40">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" t="s">
+        <v>104</v>
+      </c>
+      <c r="D41" t="s">
+        <v>105</v>
+      </c>
+      <c r="E41" t="s">
+        <v>106</v>
+      </c>
+      <c r="F41" t="s">
+        <v>107</v>
+      </c>
+      <c r="L41">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>4</v>
-      </c>
-      <c r="B41" t="s">
-        <v>103</v>
-      </c>
-      <c r="C41" t="s">
-        <v>103</v>
-      </c>
-      <c r="D41" t="s">
-        <v>104</v>
-      </c>
-      <c r="E41" t="s">
-        <v>105</v>
-      </c>
-      <c r="F41" t="s">
-        <v>106</v>
-      </c>
-      <c r="G41" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>3</v>
       </c>
       <c r="B42" t="s">
         <v>108</v>
@@ -2070,35 +2690,56 @@
         <v>108</v>
       </c>
       <c r="D42" t="s">
+        <v>108</v>
+      </c>
+      <c r="E42" t="s">
         <v>109</v>
       </c>
-      <c r="E42" t="s">
-        <v>110</v>
-      </c>
-      <c r="F42" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L42">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>4</v>
+        <f>3.5*1.75</f>
+        <v>6.125</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C43" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="D43" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="E43" t="s">
-        <v>113</v>
+        <v>118</v>
+      </c>
+      <c r="F43" t="s">
+        <v>119</v>
+      </c>
+      <c r="G43" t="s">
+        <v>118</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="L43">
+        <f>Table1[[#This Row],[Unit Price]]*Table1[[#This Row],[Qty]]</f>
+        <v>6.125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L45">
+        <f>SUM(Table1[Total Cost])</f>
+        <v>19.344999999999999</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J4" r:id="rId1" display="http://digikey.com/Suppliers/us/Lite-On.page?lang=en"/>
+    <hyperlink ref="H4" r:id="rId1" display="http://digikey.com/Suppliers/us/Lite-On.page?lang=en"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>